<commit_message>
Update Excel with full assessment text from PDF reports
- Created update_excel_with_full_reports.py script
- Extracts complete strengths and weaknesses text from student PDFs
- Updated 33/33 students with full detailed feedback
- Excel now contains full assessment text instead of just summaries

RESULTS:
- Key Strengths column: Now has full detailed strengths from PDF
- Key Weaknesses column: Now has full detailed improvements from PDF
- All 33 students with PDFs successfully updated

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Assignment1_Grading_Summary.xlsx
+++ b/Assignment1_Grading_Summary.xlsx
@@ -644,12 +644,19 @@
       <c r="I2" s="5" t="inlineStr"/>
       <c r="J2" s="3" t="inlineStr">
         <is>
-          <t>Complete PRD, 130 tests, 654 docstrings, research notebook with plots, cost analysis, 27 screenshots, good git</t>
+          <t> Complete PRD
+ 130 tests
+ 654 docstrings
+ research notebook with plots
+ cost analysis
+ 27 screenshots
+ good git</t>
         </is>
       </c>
       <c r="K2" s="3" t="inlineStr">
         <is>
-          <t>No pre-commit hooks, could improve test coverage</t>
+          <t> No pre-commit hooks
+ could improve test coverage</t>
         </is>
       </c>
     </row>
@@ -691,12 +698,20 @@
       <c r="I3" s="5" t="inlineStr"/>
       <c r="J3" s="3" t="inlineStr">
         <is>
-          <t>Good documentation (382 docstrings), FastAPI implementation, decent git (29 commits), 10 screenshots</t>
+          <t> Good documentation (382 docstrings)
+ FastAPI implementation
+ decent git (29 commits)
+ 10 screenshots</t>
         </is>
       </c>
       <c r="K3" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, minimal testing (8 tests), no CI/CD</t>
+          <t> NO research
+ NO cost analysis
+ minimal testing (8 tests)
+ no CI/CD
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -738,12 +753,20 @@
       <c r="I4" s="5" t="inlineStr"/>
       <c r="J4" s="3" t="inlineStr">
         <is>
-          <t>Good documentation (382 docstrings), FastAPI implementation, decent git (29 commits), 10 screenshots</t>
+          <t> Good documentation (382 docstrings)
+ FastAPI implementation
+ decent git (29 commits)
+ 10 screenshots</t>
         </is>
       </c>
       <c r="K4" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, minimal testing (8 tests), no CI/CD</t>
+          <t> NO research
+ NO cost analysis
+ minimal testing (8 tests)
+ no CI/CD
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -785,12 +808,19 @@
       <c r="I5" s="5" t="inlineStr"/>
       <c r="J5" s="3" t="inlineStr">
         <is>
-          <t>Complete PRD, 130 tests, 654 docstrings, research notebook with plots, cost analysis, 27 screenshots, good git</t>
+          <t> Complete PRD
+ 130 tests
+ 654 docstrings
+ research notebook with plots
+ cost analysis
+ 27 screenshots
+ good git</t>
         </is>
       </c>
       <c r="K5" s="3" t="inlineStr">
         <is>
-          <t>No pre-commit hooks, could improve test coverage</t>
+          <t> No pre-commit hooks
+ could improve test coverage</t>
         </is>
       </c>
     </row>
@@ -832,12 +862,22 @@
       <c r="I6" s="5" t="inlineStr"/>
       <c r="J6" s="3" t="inlineStr">
         <is>
-          <t>144 tests, 413 docstrings, 3062-word README, complete prompt book, budget management, 14 screenshots, 55 commits</t>
+          <t>■ 144 tests
+■ 413 docstrings
+■ 3062-word README
+■ complete prompt book
+■ budget management
+■ 14 screenshots
+■ 55 commits
+■</t>
         </is>
       </c>
       <c r="K6" s="3" t="inlineStr">
         <is>
-          <t>No research component, no pre-commit hooks</t>
+          <t> No research component
+ no pre-commit hooks
+Keep up the good work! With attention to the improvement areas noted above, you can reach the
+highest tier of performance.</t>
         </is>
       </c>
     </row>
@@ -879,12 +919,20 @@
       <c r="I7" s="5" t="inlineStr"/>
       <c r="J7" s="3" t="inlineStr">
         <is>
-          <t>Good documentation (368 docstrings), decent testing (33 tests), good git (23 commits), 7 screenshots</t>
+          <t> Good documentation (368 docstrings)
+ decent testing (33 tests)
+ good git (23 commits)
+ 7 screenshots</t>
         </is>
       </c>
       <c r="K7" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, no architecture doc, no CI/CD</t>
+          <t> NO research
+ NO cost analysis
+ no architecture doc
+ no CI/CD
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -973,12 +1021,18 @@
       <c r="I9" s="5" t="inlineStr"/>
       <c r="J9" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38955 - Good documentation, decent testing, good git</t>
+          <t> DUPLICATE of 38955 - Good documentation
+ decent testing
+ good git</t>
         </is>
       </c>
       <c r="K9" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, no architecture doc</t>
+          <t> NO research
+ NO cost analysis
+ no architecture doc
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -1020,12 +1074,23 @@
       <c r="I10" s="5" t="inlineStr"/>
       <c r="J10" s="3" t="inlineStr">
         <is>
-          <t>HIGHEST SCORE! 500 tests, 1109 docstrings (96%), 19,411-word README, dual-interface, 3 CI/CD workflows, 28 screenshots, cost analysis</t>
+          <t>■ HIGHEST SCORE! 500 tests
+■ 1109 docstrings (96%)
+■ 19
+■ 411-word README
+■ dual-interface
+■ 3 CI/CD workflows
+■ 28 screenshots
+■ cost analysis
+■</t>
         </is>
       </c>
       <c r="K10" s="3" t="inlineStr">
         <is>
-          <t>No Jupyter notebook, no pre-commit hooks</t>
+          <t> No Jupyter notebook
+ no pre-commit hooks
+Keep up the good work! With attention to the improvement areas noted above, you can reach the
+highest tier of performance.</t>
         </is>
       </c>
     </row>
@@ -1067,12 +1132,21 @@
       <c r="I11" s="5" t="inlineStr"/>
       <c r="J11" s="3" t="inlineStr">
         <is>
-          <t>144 tests, 413 docstrings, 3062-word README, complete prompt book, budget management, 14 screenshots, 55 commits</t>
+          <t>✓ 144 tests
+✓ 413 docstrings
+✓ 3062-word README
+✓ complete prompt book
+✓ budget management
+✓ 14 screenshots
+✓ 55 commits
+■</t>
         </is>
       </c>
       <c r="K11" s="3" t="inlineStr">
         <is>
-          <t>No research component, no pre-commit hooks</t>
+          <t> No research component
+ no pre-commit hooks
+Continue improving. Focus on the areas identified above to elevate your work to the next level.</t>
         </is>
       </c>
     </row>
@@ -1114,12 +1188,20 @@
       <c r="I12" s="5" t="inlineStr"/>
       <c r="J12" s="3" t="inlineStr">
         <is>
-          <t>2 comprehensive Jupyter notebooks with plots/analysis, 173 tests, excellent documentation, complete PRD, cost analysis, 16 screenshots</t>
+          <t>✓ 2 comprehensive Jupyter notebooks with plots/analysis
+✓ 173 tests
+✓ excellent documentation
+✓ complete PRD
+✓ cost analysis
+✓ 16 screenshots
+■</t>
         </is>
       </c>
       <c r="K12" s="3" t="inlineStr">
         <is>
-          <t>No pre-commit hooks, could improve CI/CD coverage</t>
+          <t> No pre-commit hooks
+ could improve CI/CD coverage
+Continue improving. Focus on the areas identified above to elevate your work to the next level.</t>
         </is>
       </c>
     </row>
@@ -1255,12 +1337,20 @@
       <c r="I15" s="5" t="inlineStr"/>
       <c r="J15" s="3" t="inlineStr">
         <is>
-          <t>Basic FastAPI implementation, 11 screenshots, decent README structure</t>
+          <t> Basic FastAPI implementation
+ 11 screenshots
+ decent README structure</t>
         </is>
       </c>
       <c r="K15" s="3" t="inlineStr">
         <is>
-          <t>NO tests, NO research, NO cost analysis, minimal documentation (38 docstrings), weak git (4 commits)</t>
+          <t> NO tests
+ NO research
+ NO cost analysis
+ minimal documentation (38 docstrings)
+ weak git (4 commits)
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -1396,12 +1486,19 @@
       <c r="I18" s="5" t="inlineStr"/>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t>Good documentation (272 docstrings), 13 screenshots, decent README (1866 words)</t>
+          <t> Good documentation (272 docstrings)
+ 13 screenshots
+ decent README (1866 words)</t>
         </is>
       </c>
       <c r="K18" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, minimal testing (12 tests), weak git (7 commits)</t>
+          <t> NO research
+ NO cost analysis
+ minimal testing (12 tests)
+ weak git (7 commits)
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -1537,12 +1634,20 @@
       <c r="I21" s="5" t="inlineStr"/>
       <c r="J21" s="3" t="inlineStr">
         <is>
-          <t>Strong testing (212 tests, 93% coverage), 441 docstrings, 6029-word README, 21 screenshots, good git (33 commits)</t>
+          <t> Strong testing (212 tests
+ 93% coverage)
+ 441 docstrings
+ 6029-word README
+ 21 screenshots
+ good git (33 commits)</t>
         </is>
       </c>
       <c r="K21" s="3" t="inlineStr">
         <is>
-          <t>No PRD, no research, no cost analysis, no pre-commit hooks</t>
+          <t> No PRD
+ no research
+ no cost analysis
+ no pre-commit hooks</t>
         </is>
       </c>
     </row>
@@ -1584,12 +1689,17 @@
       <c r="I22" s="5" t="inlineStr"/>
       <c r="J22" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38960 - 2 Jupyter notebooks, 173 tests, excellent documentation</t>
+          <t>✓ DUPLICATE of 38960 - 2 Jupyter notebooks
+✓ 173 tests
+✓ excellent documentation
+■</t>
         </is>
       </c>
       <c r="K22" s="3" t="inlineStr">
         <is>
-          <t>No pre-commit hooks, could improve CI/CD</t>
+          <t> No pre-commit hooks
+ could improve CI/CD
+Continue improving. Focus on the areas identified above to elevate your work to the next level.</t>
         </is>
       </c>
     </row>
@@ -1631,12 +1741,16 @@
       <c r="I23" s="5" t="inlineStr"/>
       <c r="J23" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38969 - 212 tests (93% coverage), 441 docstrings, 6029-word README</t>
+          <t> DUPLICATE of 38969 - 212 tests (93% coverage)
+ 441 docstrings
+ 6029-word README</t>
         </is>
       </c>
       <c r="K23" s="3" t="inlineStr">
         <is>
-          <t>No PRD, no research, no cost analysis</t>
+          <t> No PRD
+ no research
+ no cost analysis</t>
         </is>
       </c>
     </row>
@@ -1725,12 +1839,20 @@
       <c r="I25" s="5" t="inlineStr"/>
       <c r="J25" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38953 - Complete PRD, 130 tests, 654 docstrings, research notebook, cost analysis, 27 screenshots</t>
+          <t>✓ DUPLICATE of 38953 - Complete PRD
+✓ 130 tests
+✓ 654 docstrings
+✓ research notebook
+✓ cost analysis
+✓ 27 screenshots
+■</t>
         </is>
       </c>
       <c r="K25" s="3" t="inlineStr">
         <is>
-          <t>No pre-commit hooks, could improve test coverage</t>
+          <t> No pre-commit hooks
+ could improve test coverage
+Continue improving. Focus on the areas identified above to elevate your work to the next level.</t>
         </is>
       </c>
     </row>
@@ -1913,12 +2035,19 @@
       <c r="I29" s="5" t="inlineStr"/>
       <c r="J29" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38986 - Perfect docstring coverage (160/160), good security, decent git history (22 commits)</t>
+          <t> DUPLICATE of 38986 - Perfect docstring coverage (160/160)
+ good security
+ decent git history (22 commits)</t>
         </is>
       </c>
       <c r="K29" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, minimal testing (21 tests), no architecture doc</t>
+          <t> NO research
+ NO cost analysis
+ minimal testing (21 tests)
+ no architecture doc
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -2007,12 +2136,18 @@
       <c r="I31" s="5" t="inlineStr"/>
       <c r="J31" s="3" t="inlineStr">
         <is>
-          <t>10 Jupyter notebooks (exceptional research!), strong testing (91 tests), excellent documentation, comprehensive PRD</t>
+          <t>✓ 10 Jupyter notebooks (exceptional research!)
+✓ strong testing (91 tests)
+✓ excellent documentation
+✓ comprehensive PRD
+■</t>
         </is>
       </c>
       <c r="K31" s="3" t="inlineStr">
         <is>
-          <t>No cost analysis, no pre-commit hooks</t>
+          <t> No cost analysis
+ no pre-commit hooks
+Continue improving. Focus on the areas identified above to elevate your work to the next level.</t>
         </is>
       </c>
     </row>
@@ -2054,12 +2189,17 @@
       <c r="I32" s="5" t="inlineStr"/>
       <c r="J32" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38979 - 10 Jupyter notebooks, 91 tests, excellent documentation</t>
+          <t>✓ DUPLICATE of 38979 - 10 Jupyter notebooks
+✓ 91 tests
+✓ excellent documentation
+■</t>
         </is>
       </c>
       <c r="K32" s="3" t="inlineStr">
         <is>
-          <t>No cost analysis, no pre-commit hooks</t>
+          <t> No cost analysis
+ no pre-commit hooks
+Continue improving. Focus on the areas identified above to elevate your work to the next level.</t>
         </is>
       </c>
     </row>
@@ -2101,12 +2241,23 @@
       <c r="I33" s="5" t="inlineStr"/>
       <c r="J33" s="3" t="inlineStr">
         <is>
-          <t>HIGHEST SCORE! 500 tests, 1109 docstrings (96%), 19,411-word README, dual-interface (Streamlit+Flask), 3 CI/CD workflows, 28 screenshots, complete cost analysis</t>
+          <t>■ HIGHEST SCORE! 500 tests
+■ 1109 docstrings (96%)
+■ 19
+■ 411-word README
+■ dual-interface (Streamlit+Flask)
+■ 3 CI/CD workflows
+■ 28 screenshots
+■ complete cost analysis
+■</t>
         </is>
       </c>
       <c r="K33" s="3" t="inlineStr">
         <is>
-          <t>No Jupyter notebook (only gap), no pre-commit hooks</t>
+          <t> No Jupyter notebook (only gap)
+ no pre-commit hooks
+■ Keep up the amazing work! This submission demonstrates mastery of software engineering
+principles and would be competitive in a professional setting. ■</t>
         </is>
       </c>
     </row>
@@ -2148,12 +2299,20 @@
       <c r="I34" s="5" t="inlineStr"/>
       <c r="J34" s="3" t="inlineStr">
         <is>
-          <t>Has Jupyter notebook with plots (rare!), 3 ADRs, good git with 4 feature branches, 259 docstrings, complete prompt book</t>
+          <t> Has Jupyter notebook with plots (rare!)
+ 3 ADRs
+ good git with 4 feature branches
+ 259 docstrings
+ complete prompt book</t>
         </is>
       </c>
       <c r="K34" s="3" t="inlineStr">
         <is>
-          <t>No cost analysis, minimal testing (23 tests), no CI/CD</t>
+          <t> No cost analysis
+ minimal testing (23 tests)
+ no CI/CD
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -2242,12 +2401,19 @@
       <c r="I36" s="5" t="inlineStr"/>
       <c r="J36" s="3" t="inlineStr">
         <is>
-          <t>Basic implementation with 11 screenshots, some documentation (142 docstrings)</t>
+          <t> Basic implementation with 11 screenshots
+ some documentation (142 docstrings)</t>
         </is>
       </c>
       <c r="K36" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, NO tests, poor security (hardcoded secrets), weak git (8 commits)</t>
+          <t> NO research
+ NO cost analysis
+ NO tests
+ poor security (hardcoded secrets)
+ weak git (8 commits)
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -2289,12 +2455,18 @@
       <c r="I37" s="5" t="inlineStr"/>
       <c r="J37" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38964 - Basic Flask implementation, 9 screenshots</t>
+          <t> DUPLICATE of 38964 - Basic Flask implementation
+ 9 screenshots</t>
         </is>
       </c>
       <c r="K37" s="3" t="inlineStr">
         <is>
-          <t>NO tests, NO research, NO architecture docs, minimal documentation</t>
+          <t> NO tests
+ NO research
+ NO architecture docs
+ minimal documentation
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -2336,12 +2508,20 @@
       <c r="I38" s="5" t="inlineStr"/>
       <c r="J38" s="3" t="inlineStr">
         <is>
-          <t>Perfect docstring coverage (160/160 = 100%), good security, decent git (22 commits), 7 screenshots</t>
+          <t> Perfect docstring coverage (160/160 = 100%)
+ good security
+ decent git (22 commits)
+ 7 screenshots</t>
         </is>
       </c>
       <c r="K38" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, minimal testing (21 tests), no architecture doc</t>
+          <t> NO research
+ NO cost analysis
+ minimal testing (21 tests)
+ no architecture doc
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -2383,12 +2563,17 @@
       <c r="I39" s="5" t="inlineStr"/>
       <c r="J39" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38953 - Complete PRD, 130 tests, 654 docstrings, research notebook, cost analysis</t>
+          <t> DUPLICATE of 38953 - Complete PRD
+ 130 tests
+ 654 docstrings
+ research notebook
+ cost analysis</t>
         </is>
       </c>
       <c r="K39" s="3" t="inlineStr">
         <is>
-          <t>No pre-commit hooks, could improve test coverage</t>
+          <t> No pre-commit hooks
+ could improve test coverage</t>
         </is>
       </c>
     </row>
@@ -2430,12 +2615,17 @@
       <c r="I40" s="5" t="inlineStr"/>
       <c r="J40" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38953 - Complete PRD, 130 tests, 654 docstrings, research notebook, cost analysis</t>
+          <t> DUPLICATE of 38953 - Complete PRD
+ 130 tests
+ 654 docstrings
+ research notebook
+ cost analysis</t>
         </is>
       </c>
       <c r="K40" s="3" t="inlineStr">
         <is>
-          <t>No pre-commit hooks, could improve test coverage</t>
+          <t> No pre-commit hooks
+ could improve test coverage</t>
         </is>
       </c>
     </row>
@@ -2477,12 +2667,18 @@
       <c r="I41" s="5" t="inlineStr"/>
       <c r="J41" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38963 - Basic FastAPI implementation, 11 screenshots</t>
+          <t> DUPLICATE of 38963 - Basic FastAPI implementation
+ 11 screenshots</t>
         </is>
       </c>
       <c r="K41" s="3" t="inlineStr">
         <is>
-          <t>NO tests, NO research, NO cost analysis, minimal documentation</t>
+          <t> NO tests
+ NO research
+ NO cost analysis
+ minimal documentation
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -2524,12 +2720,18 @@
       <c r="I42" s="5" t="inlineStr"/>
       <c r="J42" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38986 - Perfect docstring coverage (160/160), good security, decent git</t>
+          <t> DUPLICATE of 38986 - Perfect docstring coverage (160/160)
+ good security
+ decent git</t>
         </is>
       </c>
       <c r="K42" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, minimal testing (21 tests)</t>
+          <t> NO research
+ NO cost analysis
+ minimal testing (21 tests)
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -2571,12 +2773,18 @@
       <c r="I43" s="5" t="inlineStr"/>
       <c r="J43" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38982 - Has Jupyter notebook with plots, 3 ADRs, good git with feature branches</t>
+          <t> DUPLICATE of 38982 - Has Jupyter notebook with plots
+ 3 ADRs
+ good git with feature branches</t>
         </is>
       </c>
       <c r="K43" s="3" t="inlineStr">
         <is>
-          <t>No cost analysis, minimal testing, no CI/CD</t>
+          <t> No cost analysis
+ minimal testing
+ no CI/CD
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -2618,12 +2826,18 @@
       <c r="I44" s="5" t="inlineStr"/>
       <c r="J44" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38952 - Good documentation (382 docstrings), FastAPI implementation, 29 commits</t>
+          <t> DUPLICATE of 38952 - Good documentation (382 docstrings)
+ FastAPI implementation
+ 29 commits</t>
         </is>
       </c>
       <c r="K44" s="3" t="inlineStr">
         <is>
-          <t>NO research, NO cost analysis, minimal testing (8 tests)</t>
+          <t> NO research
+ NO cost analysis
+ minimal testing (8 tests)
+Please review the requirements and resubmit. Please review course materials and requirements
+carefully before your next submission.</t>
         </is>
       </c>
     </row>
@@ -2665,12 +2879,19 @@
       <c r="I45" s="5" t="inlineStr"/>
       <c r="J45" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38959 - 144 tests, 413 docstrings, complete prompt book, budget management, 14 screenshots</t>
+          <t>✓ DUPLICATE of 38959 - 144 tests
+✓ 413 docstrings
+✓ complete prompt book
+✓ budget management
+✓ 14 screenshots
+■</t>
         </is>
       </c>
       <c r="K45" s="3" t="inlineStr">
         <is>
-          <t>No research component, no pre-commit hooks</t>
+          <t> No research component
+ no pre-commit hooks
+Continue improving. Focus on the areas identified above to elevate your work to the next level.</t>
         </is>
       </c>
     </row>
@@ -2712,12 +2933,18 @@
       <c r="I46" s="5" t="inlineStr"/>
       <c r="J46" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38969 - 212 tests (93% coverage), 441 docstrings, 6029-word README, 21 screenshots</t>
+          <t> DUPLICATE of 38969 - 212 tests (93% coverage)
+ 441 docstrings
+ 6029-word README
+ 21 screenshots</t>
         </is>
       </c>
       <c r="K46" s="3" t="inlineStr">
         <is>
-          <t>No PRD, no research, no cost analysis, no pre-commit hooks</t>
+          <t> No PRD
+ no research
+ no cost analysis
+ no pre-commit hooks</t>
         </is>
       </c>
     </row>
@@ -2759,12 +2986,21 @@
       <c r="I47" s="5" t="inlineStr"/>
       <c r="J47" s="3" t="inlineStr">
         <is>
-          <t>DUPLICATE of 38981 - HIGHEST SCORE! 500 tests, 1109 docstrings, 19,411-word README, dual-interface, 3 CI/CD workflows</t>
+          <t>■ DUPLICATE of 38981 - HIGHEST SCORE! 500 tests
+■ 1109 docstrings
+■ 19
+■ 411-word README
+■ dual-interface
+■ 3 CI/CD workflows
+■</t>
         </is>
       </c>
       <c r="K47" s="3" t="inlineStr">
         <is>
-          <t>No Jupyter notebook, no pre-commit hooks</t>
+          <t> No Jupyter notebook
+ no pre-commit hooks
+■ Keep up the amazing work! This submission demonstrates mastery of software engineering
+principles and would be competitive in a professional setting. ■</t>
         </is>
       </c>
     </row>

</xml_diff>